<commit_message>
Import of DDICK/Spreadsheet-CSV-0.15 from CPAN.
gitpan-cpan-distribution: Spreadsheet-CSV
gitpan-cpan-version:      0.15
gitpan-cpan-path:         DDICK/Spreadsheet-CSV-0.15.tar.gz
gitpan-cpan-author:       DDICK
gitpan-cpan-maturity:     released
</commit_message>
<xml_diff>
--- a/t/data/sample.xlsx
+++ b/t/data/sample.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="12525"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="14370"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sample" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -19,126 +19,427 @@
     <t>Product Code</t>
   </si>
   <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>List Price Type</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>List Price Currency</t>
+  </si>
+  <si>
+    <t>List Price Unit</t>
+  </si>
+  <si>
+    <t>Amount per List Price Unit</t>
+  </si>
+  <si>
+    <t>Purchase Price Type</t>
+  </si>
+  <si>
+    <t>Purchase Price</t>
+  </si>
+  <si>
+    <t>Purchase Price Currency</t>
+  </si>
+  <si>
+    <t>Purchase Price Unit</t>
+  </si>
+  <si>
+    <t>Amount per Purchase Price Unit</t>
+  </si>
+  <si>
+    <t>Batch Level Tracking</t>
+  </si>
+  <si>
+    <t>Tax Category</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>WIDGET1</t>
   </si>
   <si>
+    <t>Exclusive</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>EACH</t>
+  </si>
+  <si>
+    <t>Inclusive</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>BOX10</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>GST</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
     <t>Amazing-PIPE!</t>
   </si>
   <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>Super Cool Widget!</t>
-  </si>
-  <si>
-    <t>There is nothing this Pipe cannot do!</t>
-  </si>
-  <si>
-    <t>List Price Type</t>
-  </si>
-  <si>
-    <t>Exclusive</t>
-  </si>
-  <si>
-    <t>List Price</t>
-  </si>
-  <si>
-    <t>List Price Currency</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
     <t>JPY</t>
   </si>
   <si>
-    <t>List Price Unit</t>
-  </si>
-  <si>
-    <t>EACH</t>
-  </si>
-  <si>
     <t>cm</t>
   </si>
   <si>
-    <t>Amount per List Price Unit</t>
-  </si>
-  <si>
-    <t>Purchase Price Type</t>
-  </si>
-  <si>
-    <t>Inclusive</t>
-  </si>
-  <si>
-    <t>Purchase Price</t>
-  </si>
-  <si>
-    <t>Purchase Price Currency</t>
-  </si>
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
-    <t>Purchase Price Unit</t>
-  </si>
-  <si>
-    <t>BOX10</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>Amount per Purchase Price Unit</t>
-  </si>
-  <si>
-    <t>Batch Level Tracking</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Tax Category</t>
-  </si>
-  <si>
-    <t>GST</t>
-  </si>
-  <si>
     <t>EXEMPT</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Active</t>
+    <t>Super Cool _x000D_
+Widget!</t>
+  </si>
+  <si>
+    <t>There is nothing this Pipe
+_x000D_ cannot do!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+  <fonts count="18" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -146,16 +447,207 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -457,82 +949,85 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B7" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>20.54</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I2">
         <v>10.54</v>
@@ -541,119 +1036,69 @@
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L2">
         <v>10</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="O2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>100000</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="I3">
         <v>2.23</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="L3">
         <v>1000</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="N3" t="s">
         <v>30</v>
       </c>
       <c r="O3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Product Code" prompt="A unique code to identify the Product" sqref="A2:A25001">
-      <formula1>35</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Product Name" prompt="A brief description of the Product" sqref="B2:B25001">
-      <formula1>50</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="List Price Type" prompt="Is the List Price for this Product Exclusive or Inclusive of Tax?" sqref="C2:C25001">
-      <formula1>"Exclusive,Inclusive"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="List Price" prompt="The List Price of the Product (What the Customer will be quoted/invoiced for)" sqref="D2:D25001">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="List Price Currency" prompt="The Currency Code for the List Price" sqref="E2:E25001">
-      <formula1>"AUD,EUR,JPY,NZD,USD"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="List Price Unit" prompt="A unique code for the Unit of Measure for the List Price" sqref="F2:F25001">
-      <formula1>15</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amount per List Price Unit" prompt="The Amount of individual Product contained in every List Price Unit" sqref="G2:G25001">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase Price Type" prompt="Is the Purchase Price for this Product Exclusive or Inclusive of Tax?" sqref="H2:H25001">
-      <formula1>"Exclusive,Inclusive"</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase Price" prompt="The Purchase Price of the Product (What the Supplier will be paid)" sqref="I2:I25001">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase Price Currency" prompt="The Currency Code for the Purchase Price" sqref="J2:J25001">
-      <formula1>"AUD,EUR,JPY,NZD,USD"</formula1>
-    </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Purchase Price Unit" prompt="The Unit of Measure for the List Price" sqref="K2:K25001">
-      <formula1>15</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amount per Purchase Price Unit" prompt="The Amount of individual Product contained in every Purchase Price Unit" sqref="L2:L25001">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Batch Level Tracking" prompt="Does this Product require to be tracked on a Batch Level through the Warehouse.  This should only be required for Product with an Expiry Date" sqref="M1:M25001">
-      <formula1>"No,Yes"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tax Category" prompt="What Category does the Product belong to for Tax purposes?" sqref="N1:N25001">
-      <formula1>"GST,EXEMPT"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Status" prompt="An Active status means the Product may be used, the Cancelled status means it may not" sqref="O1:O25001">
-      <formula1>"Active,Cancelled"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <printOptions gridLines="1" gridLinesSet="0"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait"/>
-  <headerFooter alignWithMargins="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>